<commit_message>
1. Add to javascript lib and java lib. 2. Rename java reference 3. Add rpg code reference
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Language</t>
   </si>
@@ -59,6 +59,59 @@
   </si>
   <si>
     <t>CRTSRCPF FILE(YMYLES/TESTSRC) RCDLEN(118)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0001.00 /************************************************************************/  
+0002.00 /* REFERENCE NO. : CHG-0   -16 (D6   )                                  */  
+0003.00 /* AUTHOR        : Myles Ieong                                          */  
+0004.00 /* USER ID.      : BI77PGM                                              */  
+0005.00 /* DATE WRITTEN  : 29 Mar 2016                                          */  
+0006.00 /* DESCRPITION   : Call LNSTEXTC and LNSTCTR to generate file for user  */  
+0007.00 /*                 to download and process                              */  
+0008.00 /*                                                                      */  
+0009.00 /************************************************************************/  
+0010.00          PGM                                                                
+0011.00              /* DEFINE LIBRARIES */                                         
+0012.00              DCL        VAR(&amp;YMYLES) TYPE(*CHAR) LEN(10) VALUE(YMYLES)      
+0013.00              DCL        VAR(&amp;RMVYMYLES) TYPE(*CHAR) LEN(1) VALUE('Y')       
+0014.00              DCL        VAR(&amp;IMOD) TYPE(*CHAR) LEN(10) VALUE('IMODULE')     
+0015.00              DCL        VAR(&amp;RMVIMOD) TYPE(*CHAR) LEN(1) VALUE('Y')         
+0016.00              DCL        VAR(&amp;ZNOTE) TYPE(*CHAR) LEN(10) VALUE('ZNOTELIB')   
+0017.00              DCL        VAR(&amp;RMVZNOTE) TYPE(*CHAR) LEN(1) VALUE('Y')        
+0018.00                                                                             
+0019.00              /* ADD LIBRARIES */                                              
+0020.00              ADDLIBLE   LIB(&amp;YMYLES)                                          
+0021.00              MONMSG     MSGID(CPF2103) EXEC(CHGVAR VAR(&amp;RMVYMYLES) VALUE('N'))
+0022.00              ADDLIBLE   LIB(&amp;IMOD)                                            
+0023.00              MONMSG     MSGID(CPF2103) EXEC(CHGVAR VAR(&amp;RMVIMOD) VALUE('N'))  
+0024.00              ADDLIBLE   LIB(&amp;ZNOTE)                                           
+0025.00              MONMSG     MSGID(CPF2103) EXEC(CHGVAR VAR(&amp;RMVZNOTE) VALUE('N')) 
+0026.00                                                                               
+0027.00              CLRPFM LNSTPF                                                    
+0028.00              CLRPFM LNSTLCIF                                                  
+0029.00              CLRPFM LNSTSCIF                                                  
+0030.00              CLRPFM LNSTLSACC                                                 
+0031.00              CALL PGM(LNSTEXTC)                                               
+0032.00              RUNSQLSTM  SRCFILE(QLNSTSRC) SRCMBR(LNSTSQL) COMMIT(*NONE)       
+0033.00              CALL PGM(LNSTCTR)                                                
+0034.00                                                                               
+0035.00              /* REMOVE LIBRARIES */                                           
+0036.00              IF COND(&amp;RMVYMYLES *EQ 'Y') THEN(RMVLIBLE LIB(&amp;YMYLES))          
+0037.00              IF COND(&amp;RMVZNOTE *EQ 'Y') THEN(RMVLIBLE LIB(&amp;ZNOTE))            
+0038.00              IF COND(&amp;RMVIMOD *EQ 'Y') THEN(RMVLIBLE LIB(&amp;IMOD))  
+0039.00                                                                   
+0040.00              ENDPGM                                               </t>
+  </si>
+  <si>
+    <t>Standard wrapper</t>
+  </si>
+  <si>
+    <t>print code</t>
+  </si>
+  <si>
+    <t>option 6 for files;
+wjs;
+option 2 for spool; inject para w "DEV(PRTCCB) SAVE(*YES)"</t>
   </si>
 </sst>
 </file>
@@ -420,16 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C10" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -487,7 +540,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="39.75" customHeight="1"/>
+    <row r="6" spans="1:3" ht="39.75" customHeight="1">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34.5">
+      <c r="A7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add cl-lib entry abt job log
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Language</t>
   </si>
@@ -175,6 +175,13 @@
   </si>
   <si>
     <t>When running any jobs, press shift+esc-&gt;3 to the "display job" screen, then navi to 11. Display Call Stack/</t>
+  </si>
+  <si>
+    <t>Check job log</t>
+  </si>
+  <si>
+    <t>WRKUSRJOB USER(BG60) STATUS(*ACTIVE)
+Can be used to view job failure point (in my case, check time deposit level up function failure point that the authority of itrtchk &amp; itrprotyp &amp; itrmaincl)</t>
   </si>
 </sst>
 </file>
@@ -536,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
@@ -700,6 +707,17 @@
       </c>
       <c r="C14" s="4" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34.5">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add entries in index
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Language</t>
   </si>
@@ -169,19 +169,6 @@
 ...
 END:
              ENDPGM</t>
-  </si>
-  <si>
-    <t>check call stack</t>
-  </si>
-  <si>
-    <t>When running any jobs, press shift+esc-&gt;3 to the "display job" screen, then navi to 11. Display Call Stack/</t>
-  </si>
-  <si>
-    <t>Check job log</t>
-  </si>
-  <si>
-    <t>WRKUSRJOB USER(BG60) STATUS(*ACTIVE)
-Can be used to view job failure point (in my case, check time deposit level up function failure point that the authority of itrtchk &amp; itrprotyp &amp; itrmaincl)</t>
   </si>
 </sst>
 </file>
@@ -543,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -696,28 +683,6 @@
       </c>
       <c r="C13" s="4" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="23.25">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="34.5">
-      <c r="A15" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entries for python web framework, microservice architecture and aws concepts
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Language</t>
   </si>
@@ -169,6 +169,36 @@
 ...
 END:
              ENDPGM</t>
+  </si>
+  <si>
+    <t>DSPTAP 
+TAP02 
+*LABELS   &lt;--- Label option is equivalent to $ls 
+*PRINT   
+RSTOBJ 
+OBJ(CUP00301 CUP00901 CUP02701 LNP00301 TAP00201 TAP01401 TAP00101 CUP01901 CUP07001)
+SAVLIB(ICBSBCMDB1) &lt;--- library name in the tap (like the concept of folder name)
+DEV(TAP02) &lt;--- tap drive name, keep constant
+SEQNBR(xxx) &lt;--- the seq name used together with folder name(savlib) to identify the target folder
+ENDOPT(*LEAVE) &lt;--- no rewind so that next read time cost will be less
+RSTLIB(y20xx) &lt;---restore destination
+RSTOBJ 
+OBJ(ZPDCRCDC ZPDCRCUC) 
+SAVLIB(ZCLNKFIL) 
+DEV(TAP02) 
+SEQNBR(xxx) 
+ENDOPT(*LEAVE) 
+RSTLIB(y20xx)
+RSTOBJ 
+OBJ(ICBSRRTE) 
+SAVLIB(IPROD) 
+DEV(TAP02) 
+SEQNBR(xxx) 
+ENDOPT(*LEAVE) 
+RSTLIB(y20xx)</t>
+  </si>
+  <si>
+    <t>Display and restore tape</t>
   </si>
 </sst>
 </file>
@@ -530,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="A14:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,6 +713,17 @@
       </c>
       <c r="C13" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="63" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add index entry on rpg programming, and add journal usage in cl_lib
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Language</t>
   </si>
@@ -199,6 +199,24 @@
   </si>
   <si>
     <t>Display and restore tape</t>
+  </si>
+  <si>
+    <t>Journaling</t>
+  </si>
+  <si>
+    <t>Basic Demo</t>
+  </si>
+  <si>
+    <t>#1. Create a journal receiver: 
+        $ CRTJRNRCV JRNRCV(MYLIB/JRNRCV0001)
+#2. Create a journal: 
+        $ CRTJRN JRN(MYLIB/JOURNAL) JRNRCV(MYLIB/JRNRCV0001) MINENTDTA(*NONE)
+#3. Start journaling the file to the journal:
+        $ STRJRNPF FILE(MYLIB/CUSTOMERS) JRN(MYLIB/JOURNAL)
+            IMAGES(*BOTH) OMTJRNE(*OPNCLO)
+#4. Display and dump the journal of the file:
+        $ DSPJRN JRN(YMYLES/JOURNAL) FILE((YMYLES/CUSTOMERS)) OUTPUT(*PRINT)
+(p.s A journal can take more than 1 file at the same time)</t>
   </si>
 </sst>
 </file>
@@ -560,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -724,6 +742,17 @@
       </c>
       <c r="C14" s="4" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="113.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cl entry on pf members manipulation & java entry on using file stream
</commit_message>
<xml_diff>
--- a/cl_lib.xlsx
+++ b/cl_lib.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t>Language</t>
   </si>
@@ -217,6 +217,55 @@
 #4. Display and dump the journal of the file:
         $ DSPJRN JRN(YMYLES/JOURNAL) FILE((YMYLES/CUSTOMERS)) OUTPUT(*PRINT)
 (p.s A journal can take more than 1 file at the same time)</t>
+  </si>
+  <si>
+    <t>CPF0886</t>
+  </si>
+  <si>
+    <t>RCVF Error</t>
+  </si>
+  <si>
+    <t>Rason: The record read into CL contains not valid field (maybe too long)
+Senario: ZCHQLIB/CQRXCL read CQRXBRN cause CPF0886, to solve the error, change all S decimal in CQRXBRN to P….</t>
+  </si>
+  <si>
+    <t>OVRDBF to diff members</t>
+  </si>
+  <si>
+    <t>PF members</t>
+  </si>
+  <si>
+    <t>OVRDBF FILE(OVLNDATA) TOFILE(*LIBL/OVLNDATA) MBR(OVLNDATA1)
+DLTOVR *ALL</t>
+  </si>
+  <si>
+    <t>Add new members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDPFM FILE(ZCHQLIB/CQRXIN) MBR(M008) TEXT('Kin Wa Branch') </t>
+  </si>
+  <si>
+    <t>Use SQL to search at a temp manner:
+    1. create alias myalias1 for zchqlib.cqrxin(m001) &gt; Alias MYALIAS1 created in ZCHQLIB.                  
+    2. select * from myalias1 &gt; SELECT statement run complete.</t>
+  </si>
+  <si>
+    <t>SQL query</t>
+  </si>
+  <si>
+    <t>RCVF</t>
+  </si>
+  <si>
+    <t>LOOP:      RCVF                                                       
+           MONMSG     MSGID(CPF0864) EXEC(GOTO CMDLBL(NEXT))          
+           /* Extract file CQRXCHQ */                                 
+           OVRDBF     FILE(CQRXIN) TOFILE(*LIBL/CQRXIN) MBR(&amp;CXBMBR)  
+           CALL       PGM(CQRXEXTCHQ) PARM(&amp;CXBBRN)                   
+           DLTOVR     FILE(CQRXIN)                                    
+           GOTO       CMDLBL(LOOP)                                    
+NEXT:      /* Extract file CQRXSYS */                                        
+           RUNSQLSTM  SRCFILE(&amp;WRKLIB/QCQRSRC) SRCMBR(CQRXSQL) COMMIT(*NONE) 
+          ...</t>
   </si>
 </sst>
 </file>
@@ -272,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -282,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -578,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -755,8 +807,64 @@
         <v>34</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="147">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>